<commit_message>
Made division for each score
</commit_message>
<xml_diff>
--- a/JTS_score_data.xlsx
+++ b/JTS_score_data.xlsx
@@ -542,37 +542,37 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>50025</v>
+        <v>50.025</v>
       </c>
       <c r="G2" t="n">
-        <v>91</v>
+        <v>9.1</v>
       </c>
       <c r="H2" t="n">
-        <v>94</v>
+        <v>9.4</v>
       </c>
       <c r="I2" t="n">
-        <v>93</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>93</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K2" t="n">
-        <v>91</v>
+        <v>9.1</v>
       </c>
       <c r="L2" t="n">
-        <v>92</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="M2" t="n">
-        <v>186</v>
+        <v>18.6</v>
       </c>
       <c r="N2" t="n">
-        <v>16725</v>
+        <v>16.725</v>
       </c>
       <c r="O2" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="P2" t="n">
-        <v>970</v>
+        <v>9.699999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -602,37 +602,37 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>54235</v>
+        <v>54.235</v>
       </c>
       <c r="G3" t="n">
-        <v>84</v>
+        <v>8.4</v>
       </c>
       <c r="H3" t="n">
-        <v>79</v>
+        <v>7.9</v>
       </c>
       <c r="I3" t="n">
-        <v>83</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="J3" t="n">
-        <v>81</v>
+        <v>8.1</v>
       </c>
       <c r="K3" t="n">
-        <v>79</v>
+        <v>7.9</v>
       </c>
       <c r="L3" t="n">
-        <v>79</v>
+        <v>7.9</v>
       </c>
       <c r="M3" t="n">
-        <v>161</v>
+        <v>16.1</v>
       </c>
       <c r="N3" t="n">
-        <v>15935</v>
+        <v>15.935</v>
       </c>
       <c r="O3" t="n">
-        <v>128</v>
+        <v>12.8</v>
       </c>
       <c r="P3" t="n">
-        <v>940</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="4">
@@ -662,37 +662,37 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>47785</v>
+        <v>47.785</v>
       </c>
       <c r="G4" t="n">
-        <v>91</v>
+        <v>9.1</v>
       </c>
       <c r="H4" t="n">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="I4" t="n">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="J4" t="n">
-        <v>88</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="K4" t="n">
-        <v>84</v>
+        <v>8.4</v>
       </c>
       <c r="L4" t="n">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="M4" t="n">
-        <v>179</v>
+        <v>17.9</v>
       </c>
       <c r="N4" t="n">
-        <v>15785</v>
+        <v>15.785</v>
       </c>
       <c r="O4" t="n">
-        <v>46</v>
+        <v>4.6</v>
       </c>
       <c r="P4" t="n">
-        <v>950</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="5">
@@ -722,37 +722,37 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>20130</v>
+        <v>20.13</v>
       </c>
       <c r="G5" t="n">
-        <v>31</v>
+        <v>3.1</v>
       </c>
       <c r="H5" t="n">
-        <v>34</v>
+        <v>3.4</v>
       </c>
       <c r="I5" t="n">
-        <v>34</v>
+        <v>3.4</v>
       </c>
       <c r="J5" t="n">
-        <v>33</v>
+        <v>3.3</v>
       </c>
       <c r="K5" t="n">
-        <v>33</v>
+        <v>3.3</v>
       </c>
       <c r="L5" t="n">
-        <v>34</v>
+        <v>3.4</v>
       </c>
       <c r="M5" t="n">
-        <v>67</v>
+        <v>6.7</v>
       </c>
       <c r="N5" t="n">
-        <v>6530</v>
+        <v>6.53</v>
       </c>
       <c r="O5" t="n">
-        <v>31</v>
+        <v>3.1</v>
       </c>
       <c r="P5" t="n">
-        <v>380</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="6">
@@ -782,37 +782,37 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>52320</v>
+        <v>52.32</v>
       </c>
       <c r="G6" t="n">
-        <v>79</v>
+        <v>7.9</v>
       </c>
       <c r="H6" t="n">
-        <v>83</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>86</v>
+        <v>8.6</v>
       </c>
       <c r="J6" t="n">
-        <v>84</v>
+        <v>8.4</v>
       </c>
       <c r="K6" t="n">
-        <v>83</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="L6" t="n">
-        <v>84</v>
+        <v>8.4</v>
       </c>
       <c r="M6" t="n">
-        <v>168</v>
+        <v>16.8</v>
       </c>
       <c r="N6" t="n">
-        <v>15020</v>
+        <v>15.02</v>
       </c>
       <c r="O6" t="n">
-        <v>111</v>
+        <v>11.1</v>
       </c>
       <c r="P6" t="n">
-        <v>940</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="7">
@@ -842,37 +842,37 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>30990</v>
+        <v>30.99</v>
       </c>
       <c r="G7" t="n">
-        <v>47</v>
+        <v>4.7</v>
       </c>
       <c r="H7" t="n">
-        <v>54</v>
+        <v>5.4</v>
       </c>
       <c r="I7" t="n">
-        <v>51</v>
+        <v>5.1</v>
       </c>
       <c r="J7" t="n">
-        <v>49</v>
+        <v>4.9</v>
       </c>
       <c r="K7" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="L7" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="M7" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N7" t="n">
-        <v>9190</v>
+        <v>9.19</v>
       </c>
       <c r="O7" t="n">
-        <v>68</v>
+        <v>6.8</v>
       </c>
       <c r="P7" t="n">
-        <v>500</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -902,37 +902,37 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>35870</v>
+        <v>35.87</v>
       </c>
       <c r="G8" t="n">
-        <v>58</v>
+        <v>5.8</v>
       </c>
       <c r="H8" t="n">
-        <v>57</v>
+        <v>5.7</v>
       </c>
       <c r="I8" t="n">
-        <v>57</v>
+        <v>5.7</v>
       </c>
       <c r="J8" t="n">
-        <v>57</v>
+        <v>5.7</v>
       </c>
       <c r="K8" t="n">
-        <v>57</v>
+        <v>5.7</v>
       </c>
       <c r="L8" t="n">
-        <v>56</v>
+        <v>5.6</v>
       </c>
       <c r="M8" t="n">
-        <v>114</v>
+        <v>11.4</v>
       </c>
       <c r="N8" t="n">
-        <v>10470</v>
+        <v>10.47</v>
       </c>
       <c r="O8" t="n">
-        <v>75</v>
+        <v>7.5</v>
       </c>
       <c r="P8" t="n">
-        <v>650</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="9">
@@ -962,37 +962,37 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>49615</v>
+        <v>49.615</v>
       </c>
       <c r="G9" t="n">
-        <v>81</v>
+        <v>8.1</v>
       </c>
       <c r="H9" t="n">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="I9" t="n">
-        <v>82</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>85</v>
+        <v>8.5</v>
       </c>
       <c r="K9" t="n">
-        <v>81</v>
+        <v>8.1</v>
       </c>
       <c r="L9" t="n">
-        <v>81</v>
+        <v>8.1</v>
       </c>
       <c r="M9" t="n">
-        <v>162</v>
+        <v>16.2</v>
       </c>
       <c r="N9" t="n">
-        <v>15615</v>
+        <v>15.615</v>
       </c>
       <c r="O9" t="n">
-        <v>86</v>
+        <v>8.6</v>
       </c>
       <c r="P9" t="n">
-        <v>920</v>
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1022,37 +1022,37 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>50585</v>
+        <v>50.585</v>
       </c>
       <c r="G10" t="n">
-        <v>83</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="I10" t="n">
-        <v>84</v>
+        <v>8.4</v>
       </c>
       <c r="J10" t="n">
-        <v>82</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="K10" t="n">
-        <v>84</v>
+        <v>8.4</v>
       </c>
       <c r="L10" t="n">
-        <v>85</v>
+        <v>8.5</v>
       </c>
       <c r="M10" t="n">
-        <v>165</v>
+        <v>16.5</v>
       </c>
       <c r="N10" t="n">
-        <v>15585</v>
+        <v>15.585</v>
       </c>
       <c r="O10" t="n">
-        <v>88</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="P10" t="n">
-        <v>970</v>
+        <v>9.699999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>